<commit_message>
Mise en https de l'étape 2
</commit_message>
<xml_diff>
--- a/documentation/Recette Client.xlsx
+++ b/documentation/Recette Client.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Recette Client" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="117">
   <si>
     <t>Id Exigence</t>
   </si>
@@ -264,11 +264,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>Contrôles dates via JS puis Symfony.
-Pas de contrôle des jours fériés.
-Contrôle de non dépassement de la capacité du musé via AJAX sur la 1ère page.</t>
-  </si>
-  <si>
     <t>Pour chaque billet, l’utilisateur doit indiquer son nom, son prénom, son pays et sa
 date de naissance. Elle déterminera le tarif du billet.</t>
   </si>
@@ -411,12 +406,42 @@
     <t>Arborescence Projet.graphml
 Arborescence Projet.pdf</t>
   </si>
+  <si>
+    <t xml:space="preserve">Ce document n'a pas été établit. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Contrôles dates via JS puis Symfony.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pas de contrôle des jours fériés.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Contrôle de non dépassement de la capacité du musé via AJAX sur la 1ère page.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,6 +489,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -661,59 +693,59 @@
     <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1035,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,13 +1082,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1179,7 +1211,7 @@
       <c r="B9" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -1189,7 +1221,7 @@
     <row r="10" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="25"/>
-      <c r="C10" s="23"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="7" t="s">
         <v>55</v>
       </c>
@@ -1208,15 +1240,15 @@
         <v>22</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>11</v>
@@ -1225,15 +1257,15 @@
         <v>22</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>72</v>
@@ -1242,7 +1274,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1256,10 +1288,10 @@
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>11</v>
@@ -1268,15 +1300,15 @@
         <v>22</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>11</v>
@@ -1285,15 +1317,15 @@
         <v>22</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>11</v>
@@ -1304,10 +1336,10 @@
     </row>
     <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>72</v>
@@ -1316,15 +1348,15 @@
         <v>22</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>72</v>
@@ -1333,17 +1365,17 @@
         <v>22</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -1353,57 +1385,57 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="25"/>
-      <c r="C21" s="23"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="32" t="s">
         <v>100</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>101</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="20"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="25"/>
       <c r="C23" s="33"/>
       <c r="D23" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E23" s="21"/>
+        <v>96</v>
+      </c>
+      <c r="E23" s="35"/>
     </row>
     <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -1413,17 +1445,17 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="25"/>
-      <c r="C26" s="23"/>
+      <c r="C26" s="31"/>
       <c r="D26" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>72</v>
@@ -1431,8 +1463,8 @@
       <c r="D27" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="30" t="s">
-        <v>108</v>
+      <c r="E27" s="36" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1440,12 +1472,26 @@
       <c r="B28" s="25"/>
       <c r="C28" s="29"/>
       <c r="D28" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E28" s="31"/>
+        <v>96</v>
+      </c>
+      <c r="E28" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
@@ -1454,20 +1500,6 @@
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="E27:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1490,9 +1522,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1571,8 +1603,8 @@
       <c r="C5" s="19">
         <v>1</v>
       </c>
-      <c r="D5" s="37" t="s">
-        <v>115</v>
+      <c r="D5" s="20" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1639,10 +1671,12 @@
       <c r="B10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="16">
         <v>0</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1712,7 +1746,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1738,35 +1772,35 @@
         <v>0</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>97</v>
       </c>
       <c r="C18" s="16">
         <v>0</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>109</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="C19" s="15">
         <v>1</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Recette client et descriptif fonctionnel
</commit_message>
<xml_diff>
--- a/documentation/Recette Client.xlsx
+++ b/documentation/Recette Client.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="118">
   <si>
     <t>Id Exigence</t>
   </si>
@@ -435,6 +435,9 @@
       <t xml:space="preserve">
 Contrôle de non dépassement de la capacité du musé via AJAX sur la 1ère page.</t>
     </r>
+  </si>
+  <si>
+    <t>Action de correction de rendu Bouton Paypal et champ date de l'étape E1</t>
   </si>
 </sst>
 </file>
@@ -696,6 +699,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -704,48 +749,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1067,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,13 +1085,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1205,13 +1208,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="23" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -1219,9 +1222,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="31"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="7" t="s">
         <v>55</v>
       </c>
@@ -1261,30 +1264,30 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="29" t="s">
         <v>72</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="25" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="29"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="25"/>
+      <c r="E14" s="26"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1369,13 +1372,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="23" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -1383,36 +1386,36 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="31"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="33" t="s">
         <v>100</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="34"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="33"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="35"/>
+      <c r="E23" s="22"/>
     </row>
     <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -1429,13 +1432,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="23" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -1443,41 +1446,55 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="31"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="29" t="s">
         <v>72</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="31" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="29"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="37"/>
+      <c r="E28" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="B25:B26"/>
@@ -1486,20 +1503,6 @@
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C9:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1523,8 +1526,8 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1757,9 +1760,11 @@
         <v>51</v>
       </c>
       <c r="C16" s="17">
-        <v>0</v>
-      </c>
-      <c r="D16" s="11"/>
+        <v>0.9</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -1769,7 +1774,7 @@
         <v>55</v>
       </c>
       <c r="C17" s="17">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>110</v>

</xml_diff>

<commit_message>
Nettoyage Bundle devenu inutile et ajout boutons facebook et twitter
</commit_message>
<xml_diff>
--- a/documentation/Recette Client.xlsx
+++ b/documentation/Recette Client.xlsx
@@ -699,56 +699,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1071,7 +1071,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,13 +1085,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1208,13 +1208,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -1222,9 +1222,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="7" t="s">
         <v>55</v>
       </c>
@@ -1264,30 +1264,30 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>72</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="24" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="30"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="26"/>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1313,7 +1313,7 @@
       <c r="B16" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -1372,13 +1372,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -1386,36 +1386,36 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="24"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="32" t="s">
         <v>100</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="21"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="34"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="33"/>
       <c r="D23" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="22"/>
+      <c r="E23" s="35"/>
     </row>
     <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -1432,13 +1432,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -1446,41 +1446,55 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="24"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="31"/>
       <c r="D26" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="28" t="s">
         <v>72</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="36" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="30"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="29"/>
       <c r="D28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="32"/>
+      <c r="E28" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
@@ -1489,20 +1503,6 @@
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="E27:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1526,8 +1526,8 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>